<commit_message>
Update usernameID and add mapping spreadsheet
- Changed the username ID from 99925 to 99909 in usernameID.txt.
- Added a new mapping spreadsheet (~$mapping.xlsx) containing user data.
</commit_message>
<xml_diff>
--- a/docX.xlsx
+++ b/docX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\8. Private\Tool\demowinformapp\demowinformapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66E4C6F0-372E-493D-87CE-8508D86329D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD531B6-4136-4C3F-87F4-AE146AEC4D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2C999869-EABC-407C-8E83-1FF6B6AABDB5}"/>
   </bookViews>
@@ -4952,7 +4952,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5071,6 +5071,14 @@
       <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="17">
@@ -5434,7 +5442,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5919,12 +5927,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6491,8 +6509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88896458-AAD4-4CC1-8A68-699B11D2A50F}">
   <dimension ref="A1:ES1215"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A44" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A41" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:BN57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="12.5"/>
@@ -11395,20 +11413,20 @@
         <v>106</v>
       </c>
       <c r="C50" s="23"/>
-      <c r="D50" s="51" t="s">
+      <c r="D50" s="176" t="s">
         <v>107</v>
       </c>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="23"/>
+      <c r="E50" s="177"/>
+      <c r="F50" s="177"/>
+      <c r="G50" s="177"/>
+      <c r="H50" s="177"/>
+      <c r="I50" s="177"/>
+      <c r="J50" s="177"/>
+      <c r="K50" s="177"/>
+      <c r="L50" s="177"/>
+      <c r="M50" s="177"/>
+      <c r="N50" s="177"/>
+      <c r="O50" s="178"/>
       <c r="P50" s="51" t="s">
         <v>108</v>
       </c>

</xml_diff>

<commit_message>
Update usernameID to reflect new user ID
</commit_message>
<xml_diff>
--- a/docX.xlsx
+++ b/docX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\8. Private\Tool\demowinformapp\demowinformapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD531B6-4136-4C3F-87F4-AE146AEC4D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C1BFE2-1E1E-4532-A83A-06BEE75DDD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2C999869-EABC-407C-8E83-1FF6B6AABDB5}"/>
   </bookViews>
@@ -5442,7 +5442,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5932,6 +5932,22 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -6509,7 +6525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88896458-AAD4-4CC1-8A68-699B11D2A50F}">
   <dimension ref="A1:ES1215"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A41" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A47" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B57" sqref="B57:BN57"/>
     </sheetView>
   </sheetViews>
@@ -11816,73 +11832,73 @@
     </row>
     <row r="53" spans="1:103" ht="13" customHeight="1">
       <c r="A53" s="6"/>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="179" t="s">
         <v>117</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="13"/>
-      <c r="S53" s="13"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="13"/>
-      <c r="V53" s="13"/>
-      <c r="W53" s="13"/>
-      <c r="X53" s="13"/>
-      <c r="Y53" s="13"/>
-      <c r="Z53" s="13"/>
-      <c r="AA53" s="13"/>
-      <c r="AB53" s="13"/>
-      <c r="AC53" s="13"/>
-      <c r="AD53" s="13"/>
-      <c r="AE53" s="13"/>
-      <c r="AF53" s="13"/>
-      <c r="AG53" s="13"/>
-      <c r="AH53" s="13"/>
-      <c r="AI53" s="13"/>
-      <c r="AJ53" s="13"/>
-      <c r="AK53" s="13"/>
-      <c r="AL53" s="13"/>
-      <c r="AM53" s="13"/>
-      <c r="AN53" s="13"/>
-      <c r="AO53" s="13"/>
-      <c r="AP53" s="13"/>
-      <c r="AQ53" s="13"/>
-      <c r="AR53" s="13"/>
-      <c r="AS53" s="13"/>
-      <c r="AT53" s="13"/>
-      <c r="AU53" s="13"/>
-      <c r="AV53" s="13"/>
-      <c r="AW53" s="13"/>
-      <c r="AX53" s="13"/>
-      <c r="AY53" s="13"/>
-      <c r="AZ53" s="13"/>
-      <c r="BA53" s="13"/>
-      <c r="BB53" s="13"/>
-      <c r="BC53" s="13"/>
-      <c r="BD53" s="13"/>
-      <c r="BE53" s="13"/>
-      <c r="BF53" s="13"/>
-      <c r="BG53" s="13"/>
-      <c r="BH53" s="13"/>
-      <c r="BI53" s="13"/>
-      <c r="BJ53" s="13"/>
-      <c r="BK53" s="13"/>
-      <c r="BL53" s="13"/>
-      <c r="BM53" s="13"/>
-      <c r="BN53" s="59"/>
+      <c r="C53" s="180"/>
+      <c r="D53" s="180"/>
+      <c r="E53" s="180"/>
+      <c r="F53" s="180"/>
+      <c r="G53" s="180"/>
+      <c r="H53" s="180"/>
+      <c r="I53" s="180"/>
+      <c r="J53" s="180"/>
+      <c r="K53" s="180"/>
+      <c r="L53" s="180"/>
+      <c r="M53" s="180"/>
+      <c r="N53" s="180"/>
+      <c r="O53" s="180"/>
+      <c r="P53" s="180"/>
+      <c r="Q53" s="180"/>
+      <c r="R53" s="180"/>
+      <c r="S53" s="180"/>
+      <c r="T53" s="180"/>
+      <c r="U53" s="180"/>
+      <c r="V53" s="180"/>
+      <c r="W53" s="180"/>
+      <c r="X53" s="180"/>
+      <c r="Y53" s="180"/>
+      <c r="Z53" s="180"/>
+      <c r="AA53" s="180"/>
+      <c r="AB53" s="180"/>
+      <c r="AC53" s="180"/>
+      <c r="AD53" s="180"/>
+      <c r="AE53" s="180"/>
+      <c r="AF53" s="180"/>
+      <c r="AG53" s="180"/>
+      <c r="AH53" s="180"/>
+      <c r="AI53" s="180"/>
+      <c r="AJ53" s="180"/>
+      <c r="AK53" s="180"/>
+      <c r="AL53" s="180"/>
+      <c r="AM53" s="180"/>
+      <c r="AN53" s="180"/>
+      <c r="AO53" s="180"/>
+      <c r="AP53" s="180"/>
+      <c r="AQ53" s="180"/>
+      <c r="AR53" s="180"/>
+      <c r="AS53" s="180"/>
+      <c r="AT53" s="180"/>
+      <c r="AU53" s="180"/>
+      <c r="AV53" s="180"/>
+      <c r="AW53" s="180"/>
+      <c r="AX53" s="180"/>
+      <c r="AY53" s="180"/>
+      <c r="AZ53" s="180"/>
+      <c r="BA53" s="180"/>
+      <c r="BB53" s="180"/>
+      <c r="BC53" s="180"/>
+      <c r="BD53" s="180"/>
+      <c r="BE53" s="180"/>
+      <c r="BF53" s="180"/>
+      <c r="BG53" s="180"/>
+      <c r="BH53" s="180"/>
+      <c r="BI53" s="180"/>
+      <c r="BJ53" s="180"/>
+      <c r="BK53" s="180"/>
+      <c r="BL53" s="180"/>
+      <c r="BM53" s="180"/>
+      <c r="BN53" s="181"/>
       <c r="BO53" s="31"/>
       <c r="BP53" s="54" t="s">
         <v>14</v>
@@ -12171,20 +12187,20 @@
         <v>120</v>
       </c>
       <c r="C56" s="23"/>
-      <c r="D56" s="51" t="s">
+      <c r="D56" s="176" t="s">
         <v>121</v>
       </c>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="23"/>
+      <c r="E56" s="177"/>
+      <c r="F56" s="177"/>
+      <c r="G56" s="177"/>
+      <c r="H56" s="177"/>
+      <c r="I56" s="177"/>
+      <c r="J56" s="177"/>
+      <c r="K56" s="177"/>
+      <c r="L56" s="177"/>
+      <c r="M56" s="177"/>
+      <c r="N56" s="177"/>
+      <c r="O56" s="178"/>
       <c r="P56" s="51" t="s">
         <v>122</v>
       </c>
@@ -12429,73 +12445,73 @@
     </row>
     <row r="58" spans="1:103" ht="13" customHeight="1">
       <c r="A58" s="6"/>
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="179" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="13"/>
-      <c r="L58" s="13"/>
-      <c r="M58" s="13"/>
-      <c r="N58" s="13"/>
-      <c r="O58" s="13"/>
-      <c r="P58" s="13"/>
-      <c r="Q58" s="13"/>
-      <c r="R58" s="13"/>
-      <c r="S58" s="13"/>
-      <c r="T58" s="13"/>
-      <c r="U58" s="13"/>
-      <c r="V58" s="13"/>
-      <c r="W58" s="13"/>
-      <c r="X58" s="13"/>
-      <c r="Y58" s="13"/>
-      <c r="Z58" s="13"/>
-      <c r="AA58" s="13"/>
-      <c r="AB58" s="13"/>
-      <c r="AC58" s="13"/>
-      <c r="AD58" s="13"/>
-      <c r="AE58" s="13"/>
-      <c r="AF58" s="13"/>
-      <c r="AG58" s="13"/>
-      <c r="AH58" s="13"/>
-      <c r="AI58" s="13"/>
-      <c r="AJ58" s="13"/>
-      <c r="AK58" s="13"/>
-      <c r="AL58" s="13"/>
-      <c r="AM58" s="13"/>
-      <c r="AN58" s="13"/>
-      <c r="AO58" s="13"/>
-      <c r="AP58" s="13"/>
-      <c r="AQ58" s="13"/>
-      <c r="AR58" s="13"/>
-      <c r="AS58" s="13"/>
-      <c r="AT58" s="13"/>
-      <c r="AU58" s="13"/>
-      <c r="AV58" s="13"/>
-      <c r="AW58" s="13"/>
-      <c r="AX58" s="13"/>
-      <c r="AY58" s="13"/>
-      <c r="AZ58" s="13"/>
-      <c r="BA58" s="13"/>
-      <c r="BB58" s="13"/>
-      <c r="BC58" s="13"/>
-      <c r="BD58" s="13"/>
-      <c r="BE58" s="13"/>
-      <c r="BF58" s="13"/>
-      <c r="BG58" s="13"/>
-      <c r="BH58" s="13"/>
-      <c r="BI58" s="13"/>
-      <c r="BJ58" s="13"/>
-      <c r="BK58" s="13"/>
-      <c r="BL58" s="13"/>
-      <c r="BM58" s="13"/>
-      <c r="BN58" s="59"/>
+      <c r="C58" s="180"/>
+      <c r="D58" s="180"/>
+      <c r="E58" s="180"/>
+      <c r="F58" s="180"/>
+      <c r="G58" s="180"/>
+      <c r="H58" s="180"/>
+      <c r="I58" s="180"/>
+      <c r="J58" s="180"/>
+      <c r="K58" s="180"/>
+      <c r="L58" s="180"/>
+      <c r="M58" s="180"/>
+      <c r="N58" s="180"/>
+      <c r="O58" s="180"/>
+      <c r="P58" s="180"/>
+      <c r="Q58" s="180"/>
+      <c r="R58" s="180"/>
+      <c r="S58" s="180"/>
+      <c r="T58" s="180"/>
+      <c r="U58" s="180"/>
+      <c r="V58" s="180"/>
+      <c r="W58" s="180"/>
+      <c r="X58" s="180"/>
+      <c r="Y58" s="180"/>
+      <c r="Z58" s="180"/>
+      <c r="AA58" s="180"/>
+      <c r="AB58" s="180"/>
+      <c r="AC58" s="180"/>
+      <c r="AD58" s="180"/>
+      <c r="AE58" s="180"/>
+      <c r="AF58" s="180"/>
+      <c r="AG58" s="180"/>
+      <c r="AH58" s="180"/>
+      <c r="AI58" s="180"/>
+      <c r="AJ58" s="180"/>
+      <c r="AK58" s="180"/>
+      <c r="AL58" s="180"/>
+      <c r="AM58" s="180"/>
+      <c r="AN58" s="180"/>
+      <c r="AO58" s="180"/>
+      <c r="AP58" s="180"/>
+      <c r="AQ58" s="180"/>
+      <c r="AR58" s="180"/>
+      <c r="AS58" s="180"/>
+      <c r="AT58" s="180"/>
+      <c r="AU58" s="180"/>
+      <c r="AV58" s="180"/>
+      <c r="AW58" s="180"/>
+      <c r="AX58" s="180"/>
+      <c r="AY58" s="180"/>
+      <c r="AZ58" s="180"/>
+      <c r="BA58" s="180"/>
+      <c r="BB58" s="180"/>
+      <c r="BC58" s="180"/>
+      <c r="BD58" s="180"/>
+      <c r="BE58" s="180"/>
+      <c r="BF58" s="180"/>
+      <c r="BG58" s="180"/>
+      <c r="BH58" s="180"/>
+      <c r="BI58" s="180"/>
+      <c r="BJ58" s="180"/>
+      <c r="BK58" s="180"/>
+      <c r="BL58" s="180"/>
+      <c r="BM58" s="180"/>
+      <c r="BN58" s="181"/>
       <c r="BO58" s="31"/>
       <c r="BP58" s="54" t="s">
         <v>14</v>
@@ -12546,73 +12562,73 @@
     </row>
     <row r="59" spans="1:103" ht="13" customHeight="1">
       <c r="A59" s="6"/>
-      <c r="B59" s="58" t="s">
+      <c r="B59" s="179" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="13"/>
-      <c r="N59" s="13"/>
-      <c r="O59" s="13"/>
-      <c r="P59" s="13"/>
-      <c r="Q59" s="13"/>
-      <c r="R59" s="13"/>
-      <c r="S59" s="13"/>
-      <c r="T59" s="13"/>
-      <c r="U59" s="13"/>
-      <c r="V59" s="13"/>
-      <c r="W59" s="13"/>
-      <c r="X59" s="13"/>
-      <c r="Y59" s="13"/>
-      <c r="Z59" s="13"/>
-      <c r="AA59" s="13"/>
-      <c r="AB59" s="13"/>
-      <c r="AC59" s="13"/>
-      <c r="AD59" s="13"/>
-      <c r="AE59" s="13"/>
-      <c r="AF59" s="13"/>
-      <c r="AG59" s="13"/>
-      <c r="AH59" s="13"/>
-      <c r="AI59" s="13"/>
-      <c r="AJ59" s="13"/>
-      <c r="AK59" s="13"/>
-      <c r="AL59" s="13"/>
-      <c r="AM59" s="13"/>
-      <c r="AN59" s="13"/>
-      <c r="AO59" s="13"/>
-      <c r="AP59" s="13"/>
-      <c r="AQ59" s="13"/>
-      <c r="AR59" s="13"/>
-      <c r="AS59" s="13"/>
-      <c r="AT59" s="13"/>
-      <c r="AU59" s="13"/>
-      <c r="AV59" s="13"/>
-      <c r="AW59" s="13"/>
-      <c r="AX59" s="13"/>
-      <c r="AY59" s="13"/>
-      <c r="AZ59" s="13"/>
-      <c r="BA59" s="13"/>
-      <c r="BB59" s="13"/>
-      <c r="BC59" s="13"/>
-      <c r="BD59" s="13"/>
-      <c r="BE59" s="13"/>
-      <c r="BF59" s="13"/>
-      <c r="BG59" s="13"/>
-      <c r="BH59" s="13"/>
-      <c r="BI59" s="13"/>
-      <c r="BJ59" s="13"/>
-      <c r="BK59" s="13"/>
-      <c r="BL59" s="13"/>
-      <c r="BM59" s="13"/>
-      <c r="BN59" s="59"/>
+      <c r="C59" s="180"/>
+      <c r="D59" s="180"/>
+      <c r="E59" s="180"/>
+      <c r="F59" s="180"/>
+      <c r="G59" s="180"/>
+      <c r="H59" s="180"/>
+      <c r="I59" s="180"/>
+      <c r="J59" s="180"/>
+      <c r="K59" s="180"/>
+      <c r="L59" s="180"/>
+      <c r="M59" s="180"/>
+      <c r="N59" s="180"/>
+      <c r="O59" s="180"/>
+      <c r="P59" s="180"/>
+      <c r="Q59" s="180"/>
+      <c r="R59" s="180"/>
+      <c r="S59" s="180"/>
+      <c r="T59" s="180"/>
+      <c r="U59" s="180"/>
+      <c r="V59" s="180"/>
+      <c r="W59" s="180"/>
+      <c r="X59" s="180"/>
+      <c r="Y59" s="180"/>
+      <c r="Z59" s="180"/>
+      <c r="AA59" s="180"/>
+      <c r="AB59" s="180"/>
+      <c r="AC59" s="180"/>
+      <c r="AD59" s="180"/>
+      <c r="AE59" s="180"/>
+      <c r="AF59" s="180"/>
+      <c r="AG59" s="180"/>
+      <c r="AH59" s="180"/>
+      <c r="AI59" s="180"/>
+      <c r="AJ59" s="180"/>
+      <c r="AK59" s="180"/>
+      <c r="AL59" s="180"/>
+      <c r="AM59" s="180"/>
+      <c r="AN59" s="180"/>
+      <c r="AO59" s="180"/>
+      <c r="AP59" s="180"/>
+      <c r="AQ59" s="180"/>
+      <c r="AR59" s="180"/>
+      <c r="AS59" s="180"/>
+      <c r="AT59" s="180"/>
+      <c r="AU59" s="180"/>
+      <c r="AV59" s="180"/>
+      <c r="AW59" s="180"/>
+      <c r="AX59" s="180"/>
+      <c r="AY59" s="180"/>
+      <c r="AZ59" s="180"/>
+      <c r="BA59" s="180"/>
+      <c r="BB59" s="180"/>
+      <c r="BC59" s="180"/>
+      <c r="BD59" s="180"/>
+      <c r="BE59" s="180"/>
+      <c r="BF59" s="180"/>
+      <c r="BG59" s="180"/>
+      <c r="BH59" s="180"/>
+      <c r="BI59" s="180"/>
+      <c r="BJ59" s="180"/>
+      <c r="BK59" s="180"/>
+      <c r="BL59" s="180"/>
+      <c r="BM59" s="180"/>
+      <c r="BN59" s="181"/>
       <c r="BO59" s="31"/>
       <c r="BP59" s="54" t="s">
         <v>14</v>
@@ -12897,101 +12913,101 @@
     </row>
     <row r="62" spans="1:103" ht="13" customHeight="1">
       <c r="A62" s="6"/>
-      <c r="B62" s="51" t="s">
+      <c r="B62" s="176" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="23"/>
-      <c r="D62" s="51" t="s">
+      <c r="C62" s="178"/>
+      <c r="D62" s="176" t="s">
         <v>128</v>
       </c>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-      <c r="O62" s="23"/>
-      <c r="P62" s="51" t="s">
+      <c r="E62" s="177"/>
+      <c r="F62" s="177"/>
+      <c r="G62" s="177"/>
+      <c r="H62" s="177"/>
+      <c r="I62" s="177"/>
+      <c r="J62" s="177"/>
+      <c r="K62" s="177"/>
+      <c r="L62" s="177"/>
+      <c r="M62" s="177"/>
+      <c r="N62" s="177"/>
+      <c r="O62" s="178"/>
+      <c r="P62" s="176" t="s">
         <v>108</v>
       </c>
-      <c r="Q62" s="22"/>
-      <c r="R62" s="22"/>
-      <c r="S62" s="22"/>
-      <c r="T62" s="23"/>
-      <c r="U62" s="52" t="s">
+      <c r="Q62" s="177"/>
+      <c r="R62" s="177"/>
+      <c r="S62" s="177"/>
+      <c r="T62" s="178"/>
+      <c r="U62" s="182" t="s">
         <v>109</v>
       </c>
-      <c r="V62" s="23"/>
-      <c r="W62" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="X62" s="22"/>
-      <c r="Y62" s="23"/>
-      <c r="Z62" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA62" s="22"/>
-      <c r="AB62" s="22"/>
-      <c r="AC62" s="23"/>
-      <c r="AD62" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE62" s="23"/>
-      <c r="AF62" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG62" s="23"/>
-      <c r="AH62" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI62" s="23"/>
-      <c r="AJ62" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK62" s="23"/>
-      <c r="AL62" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM62" s="23"/>
-      <c r="AN62" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO62" s="22"/>
-      <c r="AP62" s="22"/>
-      <c r="AQ62" s="22"/>
-      <c r="AR62" s="22"/>
-      <c r="AS62" s="23"/>
-      <c r="AT62" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU62" s="22"/>
-      <c r="AV62" s="22"/>
-      <c r="AW62" s="22"/>
-      <c r="AX62" s="22"/>
-      <c r="AY62" s="22"/>
-      <c r="AZ62" s="23"/>
-      <c r="BA62" s="51" t="s">
+      <c r="V62" s="178"/>
+      <c r="W62" s="182" t="s">
+        <v>110</v>
+      </c>
+      <c r="X62" s="177"/>
+      <c r="Y62" s="178"/>
+      <c r="Z62" s="182" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA62" s="177"/>
+      <c r="AB62" s="177"/>
+      <c r="AC62" s="178"/>
+      <c r="AD62" s="183" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE62" s="178"/>
+      <c r="AF62" s="183" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG62" s="178"/>
+      <c r="AH62" s="183" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI62" s="178"/>
+      <c r="AJ62" s="183" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK62" s="178"/>
+      <c r="AL62" s="182" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM62" s="178"/>
+      <c r="AN62" s="182" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO62" s="177"/>
+      <c r="AP62" s="177"/>
+      <c r="AQ62" s="177"/>
+      <c r="AR62" s="177"/>
+      <c r="AS62" s="178"/>
+      <c r="AT62" s="182" t="s">
+        <v>110</v>
+      </c>
+      <c r="AU62" s="177"/>
+      <c r="AV62" s="177"/>
+      <c r="AW62" s="177"/>
+      <c r="AX62" s="177"/>
+      <c r="AY62" s="177"/>
+      <c r="AZ62" s="178"/>
+      <c r="BA62" s="176" t="s">
         <v>111</v>
       </c>
-      <c r="BB62" s="23"/>
-      <c r="BC62" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="BD62" s="22"/>
-      <c r="BE62" s="22"/>
-      <c r="BF62" s="22"/>
-      <c r="BG62" s="22"/>
-      <c r="BH62" s="22"/>
-      <c r="BI62" s="22"/>
-      <c r="BJ62" s="22"/>
-      <c r="BK62" s="22"/>
-      <c r="BL62" s="22"/>
-      <c r="BM62" s="22"/>
-      <c r="BN62" s="23"/>
+      <c r="BB62" s="178"/>
+      <c r="BC62" s="182" t="s">
+        <v>110</v>
+      </c>
+      <c r="BD62" s="177"/>
+      <c r="BE62" s="177"/>
+      <c r="BF62" s="177"/>
+      <c r="BG62" s="177"/>
+      <c r="BH62" s="177"/>
+      <c r="BI62" s="177"/>
+      <c r="BJ62" s="177"/>
+      <c r="BK62" s="177"/>
+      <c r="BL62" s="177"/>
+      <c r="BM62" s="177"/>
+      <c r="BN62" s="178"/>
       <c r="BO62" s="31"/>
       <c r="BP62" s="54" t="s">
         <v>14</v>
@@ -13042,101 +13058,101 @@
     </row>
     <row r="63" spans="1:103" ht="13" customHeight="1">
       <c r="A63" s="6"/>
-      <c r="B63" s="51" t="s">
+      <c r="B63" s="176" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="23"/>
-      <c r="D63" s="51" t="s">
+      <c r="C63" s="178"/>
+      <c r="D63" s="176" t="s">
         <v>129</v>
       </c>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
-      <c r="O63" s="23"/>
-      <c r="P63" s="51" t="s">
+      <c r="E63" s="177"/>
+      <c r="F63" s="177"/>
+      <c r="G63" s="177"/>
+      <c r="H63" s="177"/>
+      <c r="I63" s="177"/>
+      <c r="J63" s="177"/>
+      <c r="K63" s="177"/>
+      <c r="L63" s="177"/>
+      <c r="M63" s="177"/>
+      <c r="N63" s="177"/>
+      <c r="O63" s="178"/>
+      <c r="P63" s="176" t="s">
         <v>112</v>
       </c>
-      <c r="Q63" s="22"/>
-      <c r="R63" s="22"/>
-      <c r="S63" s="22"/>
-      <c r="T63" s="23"/>
-      <c r="U63" s="51" t="s">
+      <c r="Q63" s="177"/>
+      <c r="R63" s="177"/>
+      <c r="S63" s="177"/>
+      <c r="T63" s="178"/>
+      <c r="U63" s="176" t="s">
         <v>130</v>
       </c>
-      <c r="V63" s="23"/>
-      <c r="W63" s="51" t="s">
+      <c r="V63" s="178"/>
+      <c r="W63" s="176" t="s">
         <v>131</v>
       </c>
-      <c r="X63" s="22"/>
-      <c r="Y63" s="23"/>
-      <c r="Z63" s="51" t="s">
+      <c r="X63" s="177"/>
+      <c r="Y63" s="178"/>
+      <c r="Z63" s="176" t="s">
         <v>132</v>
       </c>
-      <c r="AA63" s="22"/>
-      <c r="AB63" s="22"/>
-      <c r="AC63" s="23"/>
-      <c r="AD63" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE63" s="23"/>
-      <c r="AF63" s="57">
+      <c r="AA63" s="177"/>
+      <c r="AB63" s="177"/>
+      <c r="AC63" s="178"/>
+      <c r="AD63" s="184" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE63" s="178"/>
+      <c r="AF63" s="184">
         <v>3</v>
       </c>
-      <c r="AG63" s="23"/>
-      <c r="AH63" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI63" s="23"/>
-      <c r="AJ63" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK63" s="23"/>
-      <c r="AL63" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM63" s="23"/>
-      <c r="AN63" s="51" t="s">
+      <c r="AG63" s="178"/>
+      <c r="AH63" s="184" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI63" s="178"/>
+      <c r="AJ63" s="184" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK63" s="178"/>
+      <c r="AL63" s="176" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM63" s="178"/>
+      <c r="AN63" s="176" t="s">
         <v>133</v>
       </c>
-      <c r="AO63" s="22"/>
-      <c r="AP63" s="22"/>
-      <c r="AQ63" s="22"/>
-      <c r="AR63" s="22"/>
-      <c r="AS63" s="23"/>
-      <c r="AT63" s="51" t="s">
+      <c r="AO63" s="177"/>
+      <c r="AP63" s="177"/>
+      <c r="AQ63" s="177"/>
+      <c r="AR63" s="177"/>
+      <c r="AS63" s="178"/>
+      <c r="AT63" s="176" t="s">
         <v>134</v>
       </c>
-      <c r="AU63" s="22"/>
-      <c r="AV63" s="22"/>
-      <c r="AW63" s="22"/>
-      <c r="AX63" s="22"/>
-      <c r="AY63" s="22"/>
-      <c r="AZ63" s="23"/>
-      <c r="BA63" s="51" t="s">
+      <c r="AU63" s="177"/>
+      <c r="AV63" s="177"/>
+      <c r="AW63" s="177"/>
+      <c r="AX63" s="177"/>
+      <c r="AY63" s="177"/>
+      <c r="AZ63" s="178"/>
+      <c r="BA63" s="176" t="s">
         <v>111</v>
       </c>
-      <c r="BB63" s="23"/>
-      <c r="BC63" s="51" t="s">
+      <c r="BB63" s="178"/>
+      <c r="BC63" s="176" t="s">
         <v>135</v>
       </c>
-      <c r="BD63" s="22"/>
-      <c r="BE63" s="22"/>
-      <c r="BF63" s="22"/>
-      <c r="BG63" s="22"/>
-      <c r="BH63" s="22"/>
-      <c r="BI63" s="22"/>
-      <c r="BJ63" s="22"/>
-      <c r="BK63" s="22"/>
-      <c r="BL63" s="22"/>
-      <c r="BM63" s="22"/>
-      <c r="BN63" s="23"/>
+      <c r="BD63" s="177"/>
+      <c r="BE63" s="177"/>
+      <c r="BF63" s="177"/>
+      <c r="BG63" s="177"/>
+      <c r="BH63" s="177"/>
+      <c r="BI63" s="177"/>
+      <c r="BJ63" s="177"/>
+      <c r="BK63" s="177"/>
+      <c r="BL63" s="177"/>
+      <c r="BM63" s="177"/>
+      <c r="BN63" s="178"/>
       <c r="BO63" s="31"/>
       <c r="BP63" s="54" t="s">
         <v>14</v>
@@ -13187,101 +13203,101 @@
     </row>
     <row r="64" spans="1:103" ht="13" customHeight="1">
       <c r="A64" s="6"/>
-      <c r="B64" s="51" t="s">
+      <c r="B64" s="176" t="s">
         <v>127</v>
       </c>
-      <c r="C64" s="23"/>
-      <c r="D64" s="51" t="s">
+      <c r="C64" s="178"/>
+      <c r="D64" s="176" t="s">
         <v>137</v>
       </c>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="22"/>
-      <c r="I64" s="22"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="51" t="s">
+      <c r="E64" s="177"/>
+      <c r="F64" s="177"/>
+      <c r="G64" s="177"/>
+      <c r="H64" s="177"/>
+      <c r="I64" s="177"/>
+      <c r="J64" s="177"/>
+      <c r="K64" s="177"/>
+      <c r="L64" s="177"/>
+      <c r="M64" s="177"/>
+      <c r="N64" s="177"/>
+      <c r="O64" s="178"/>
+      <c r="P64" s="176" t="s">
         <v>112</v>
       </c>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
-      <c r="S64" s="22"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="51" t="s">
+      <c r="Q64" s="177"/>
+      <c r="R64" s="177"/>
+      <c r="S64" s="177"/>
+      <c r="T64" s="178"/>
+      <c r="U64" s="176" t="s">
         <v>109</v>
       </c>
-      <c r="V64" s="23"/>
-      <c r="W64" s="51" t="s">
+      <c r="V64" s="178"/>
+      <c r="W64" s="176" t="s">
         <v>113</v>
       </c>
-      <c r="X64" s="22"/>
-      <c r="Y64" s="23"/>
-      <c r="Z64" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA64" s="22"/>
-      <c r="AB64" s="22"/>
-      <c r="AC64" s="23"/>
-      <c r="AD64" s="57">
+      <c r="X64" s="177"/>
+      <c r="Y64" s="178"/>
+      <c r="Z64" s="182" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA64" s="177"/>
+      <c r="AB64" s="177"/>
+      <c r="AC64" s="178"/>
+      <c r="AD64" s="184">
         <v>10</v>
       </c>
-      <c r="AE64" s="23"/>
-      <c r="AF64" s="57">
+      <c r="AE64" s="178"/>
+      <c r="AF64" s="184">
         <v>20</v>
       </c>
-      <c r="AG64" s="23"/>
-      <c r="AH64" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI64" s="23"/>
-      <c r="AJ64" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK64" s="23"/>
-      <c r="AL64" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM64" s="23"/>
-      <c r="AN64" s="51" t="s">
+      <c r="AG64" s="178"/>
+      <c r="AH64" s="184" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI64" s="178"/>
+      <c r="AJ64" s="184" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK64" s="178"/>
+      <c r="AL64" s="176" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM64" s="178"/>
+      <c r="AN64" s="176" t="s">
         <v>133</v>
       </c>
-      <c r="AO64" s="22"/>
-      <c r="AP64" s="22"/>
-      <c r="AQ64" s="22"/>
-      <c r="AR64" s="22"/>
-      <c r="AS64" s="23"/>
-      <c r="AT64" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU64" s="22"/>
-      <c r="AV64" s="22"/>
-      <c r="AW64" s="22"/>
-      <c r="AX64" s="22"/>
-      <c r="AY64" s="22"/>
-      <c r="AZ64" s="23"/>
-      <c r="BA64" s="51" t="s">
+      <c r="AO64" s="177"/>
+      <c r="AP64" s="177"/>
+      <c r="AQ64" s="177"/>
+      <c r="AR64" s="177"/>
+      <c r="AS64" s="178"/>
+      <c r="AT64" s="176" t="s">
+        <v>110</v>
+      </c>
+      <c r="AU64" s="177"/>
+      <c r="AV64" s="177"/>
+      <c r="AW64" s="177"/>
+      <c r="AX64" s="177"/>
+      <c r="AY64" s="177"/>
+      <c r="AZ64" s="178"/>
+      <c r="BA64" s="176" t="s">
         <v>111</v>
       </c>
-      <c r="BB64" s="23"/>
-      <c r="BC64" s="51" t="s">
+      <c r="BB64" s="178"/>
+      <c r="BC64" s="176" t="s">
         <v>138</v>
       </c>
-      <c r="BD64" s="22"/>
-      <c r="BE64" s="22"/>
-      <c r="BF64" s="22"/>
-      <c r="BG64" s="22"/>
-      <c r="BH64" s="22"/>
-      <c r="BI64" s="22"/>
-      <c r="BJ64" s="22"/>
-      <c r="BK64" s="22"/>
-      <c r="BL64" s="22"/>
-      <c r="BM64" s="22"/>
-      <c r="BN64" s="23"/>
+      <c r="BD64" s="177"/>
+      <c r="BE64" s="177"/>
+      <c r="BF64" s="177"/>
+      <c r="BG64" s="177"/>
+      <c r="BH64" s="177"/>
+      <c r="BI64" s="177"/>
+      <c r="BJ64" s="177"/>
+      <c r="BK64" s="177"/>
+      <c r="BL64" s="177"/>
+      <c r="BM64" s="177"/>
+      <c r="BN64" s="178"/>
       <c r="BO64" s="31"/>
       <c r="BP64" s="54" t="s">
         <v>14</v>

</xml_diff>